<commit_message>
Adapt ocean acidification scale
</commit_message>
<xml_diff>
--- a/data/planetary_boundaries_data.xlsx
+++ b/data/planetary_boundaries_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yeleconsultingsas-my.sharepoint.com/personal/bastien_gauthier_yele_fr/Documents/Documents/21_Chantiers_internes/Clones_git/planetary-flag/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{6B4B5E74-9189-4FFF-A8B2-D687E69AAF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF854CED-A03C-4649-9437-CE2BA434E712}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{6B4B5E74-9189-4FFF-A8B2-D687E69AAF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF5C835F-6095-4066-9A8B-E112693E8A25}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" activeTab="3" xr2:uid="{36A38DD1-033D-44E8-8F60-3212F4F44CAE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" xr2:uid="{36A38DD1-033D-44E8-8F60-3212F4F44CAE}"/>
   </bookViews>
   <sheets>
     <sheet name="synthese" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -580,7 +580,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -903,8 +903,8 @@
   </sheetPr>
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1022,10 +1022,10 @@
         <v>2.75</v>
       </c>
       <c r="H3">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L3" t="s">
         <v>60</v>
@@ -24992,7 +24992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D768F792-B1A9-4FFB-80DF-A50BE994C552}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>